<commit_message>
Bugfixing & result saving
V 1.0 complete
</commit_message>
<xml_diff>
--- a/data1.xlsx
+++ b/data1.xlsx
@@ -1,8 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
@@ -14,28 +14,56 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t>Dates</t>
-  </si>
-  <si>
-    <t>color 1</t>
-  </si>
-  <si>
-    <t>color 2</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
   <si>
     <t>jan</t>
   </si>
   <si>
     <t>feb</t>
+  </si>
+  <si>
+    <t>SIG allCap</t>
+  </si>
+  <si>
+    <t>combiCap, weiss 19099</t>
+  </si>
+  <si>
+    <t>combiCap, ecoweiss 19144</t>
+  </si>
+  <si>
+    <t>CAA</t>
+  </si>
+  <si>
+    <t>Paletten</t>
+  </si>
+  <si>
+    <t>Menge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lagerbestand Montag </t>
+  </si>
+  <si>
+    <t>älter als 6 Monate</t>
+  </si>
+  <si>
+    <t>gesperrt aus Produktion</t>
+  </si>
+  <si>
+    <t>gesperrt aus Rekl.</t>
+  </si>
+  <si>
+    <t>Produktion Datum</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="167" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="170" formatCode="dd/mm/yy;@"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -44,23 +72,48 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
+      <sz val="8"/>
+      <name val="Arial"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="22"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="43"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -77,18 +130,192 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="170" fontId="3" fillId="4" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="2" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="3" fillId="4" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="2" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="2" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="3" fillId="3" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="3" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="3" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="3" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="3" fillId="3" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="3" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="3" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="3" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="3" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="3" fillId="2" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="4">
+    <cellStyle name="Komma 2" xfId="3"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard 2" xfId="2"/>
+    <cellStyle name="Standard 3" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -390,31 +617,165 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A7:Q40"/>
+  <sheetPr codeName="Tabelle1"/>
+  <dimension ref="A1:Q40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="E2" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="5"/>
+      <c r="D1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="5"/>
+      <c r="F1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="5"/>
+    </row>
+    <row r="2" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="10">
+        <v>8</v>
+      </c>
+      <c r="C3" s="11">
+        <v>761600</v>
+      </c>
+      <c r="D3" s="10">
+        <v>88</v>
+      </c>
+      <c r="E3" s="11">
+        <v>8377600</v>
+      </c>
+      <c r="F3" s="10">
+        <v>88</v>
+      </c>
+      <c r="G3" s="11">
+        <v>8377600</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="12">
+        <v>0</v>
+      </c>
+      <c r="C4" s="11">
+        <v>0</v>
+      </c>
+      <c r="D4" s="12">
+        <v>0</v>
+      </c>
+      <c r="E4" s="11">
+        <v>0</v>
+      </c>
+      <c r="F4" s="12">
+        <v>0</v>
+      </c>
+      <c r="G4" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="12">
+        <v>0</v>
+      </c>
+      <c r="C5" s="11">
+        <v>0</v>
+      </c>
+      <c r="D5" s="12">
+        <v>0</v>
+      </c>
+      <c r="E5" s="11">
+        <v>0</v>
+      </c>
+      <c r="F5" s="12">
+        <v>0</v>
+      </c>
+      <c r="G5" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="14">
+        <v>0</v>
+      </c>
+      <c r="C6" s="15">
+        <v>0</v>
+      </c>
+      <c r="D6" s="14">
+        <v>0</v>
+      </c>
+      <c r="E6" s="15">
+        <v>0</v>
+      </c>
+      <c r="F6" s="14">
+        <v>0</v>
+      </c>
+      <c r="G6" s="15">
+        <v>0</v>
+      </c>
+    </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
+      <c r="A7" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="17"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="18"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
@@ -436,6 +797,9 @@
       <c r="E8">
         <v>8</v>
       </c>
+      <c r="G8">
+        <v>8</v>
+      </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
@@ -447,6 +811,9 @@
       <c r="E9">
         <v>8</v>
       </c>
+      <c r="G9">
+        <v>8</v>
+      </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
@@ -458,6 +825,9 @@
       <c r="E10">
         <v>48</v>
       </c>
+      <c r="G10">
+        <v>48</v>
+      </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
@@ -469,6 +839,9 @@
       <c r="E11">
         <v>464</v>
       </c>
+      <c r="G11">
+        <v>464</v>
+      </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
@@ -488,6 +861,9 @@
       <c r="E13">
         <v>24</v>
       </c>
+      <c r="G13">
+        <v>24</v>
+      </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
@@ -499,6 +875,9 @@
       <c r="E14">
         <v>1</v>
       </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
@@ -510,6 +889,9 @@
       <c r="E15">
         <v>24</v>
       </c>
+      <c r="G15">
+        <v>24</v>
+      </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
@@ -521,8 +903,11 @@
       <c r="E16">
         <v>5</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G16">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>42379</v>
       </c>
@@ -532,8 +917,11 @@
       <c r="E17">
         <v>6</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G17">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>42380</v>
       </c>
@@ -543,8 +931,11 @@
       <c r="E18">
         <v>54</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G18">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>42381</v>
       </c>
@@ -554,8 +945,11 @@
       <c r="E19">
         <v>5</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G19">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>42401</v>
       </c>
@@ -565,8 +959,11 @@
       <c r="E20">
         <v>5</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>42402</v>
       </c>
@@ -576,8 +973,11 @@
       <c r="E21">
         <v>23</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G21">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>42403</v>
       </c>
@@ -587,8 +987,11 @@
       <c r="E22">
         <v>58</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G22">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>42404</v>
       </c>
@@ -598,8 +1001,11 @@
       <c r="E23">
         <v>13</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G23">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>42405</v>
       </c>
@@ -609,8 +1015,11 @@
       <c r="E24">
         <v>8</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G24">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>42406</v>
       </c>
@@ -620,8 +1029,11 @@
       <c r="E25">
         <v>8</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>42407</v>
       </c>
@@ -631,8 +1043,11 @@
       <c r="E26">
         <v>9</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G26">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>42408</v>
       </c>
@@ -642,8 +1057,11 @@
       <c r="E27">
         <v>6</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G27">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>42430</v>
       </c>
@@ -653,8 +1071,11 @@
       <c r="E28">
         <v>4</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G28">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>42431</v>
       </c>
@@ -664,8 +1085,11 @@
       <c r="E29">
         <v>13</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G29">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>42432</v>
       </c>
@@ -675,8 +1099,11 @@
       <c r="E30">
         <v>4</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G30">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>42433</v>
       </c>
@@ -686,8 +1113,11 @@
       <c r="E31">
         <v>797</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G31">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>42434</v>
       </c>
@@ -697,8 +1127,11 @@
       <c r="E32">
         <v>8</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G32">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>42435</v>
       </c>
@@ -708,19 +1141,22 @@
       <c r="E33">
         <v>8</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G33">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C39">
-        <f>SUM(C8:C19)+SUM(E8:E19)</f>
+        <f>SUM(C8:C19)+SUM(G8:G19)</f>
         <v>2964</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C40">
         <f>SUM(C20:C27)+SUM(E20:E27)</f>
@@ -728,6 +1164,12 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="F1:G1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix: sum as Double
</commit_message>
<xml_diff>
--- a/data1.xlsx
+++ b/data1.xlsx
@@ -60,8 +60,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="167" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="170" formatCode="dd/mm/yy;@"/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="164" formatCode="dd/mm/yy;@"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -256,58 +256,58 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="170" fontId="3" fillId="4" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="4" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="4" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="2" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="2" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="3" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="3" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="3" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="3" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="3" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="3" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="3" fillId="2" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="3" fillId="4" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="3" fillId="2" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="3" fillId="2" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="3" fillId="3" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="3" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="3" fillId="3" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="3" fillId="3" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="3" fillId="3" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="3" fontId="3" fillId="3" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="3" fillId="3" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="3" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="3" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="3" fillId="2" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -621,7 +621,7 @@
   <dimension ref="A1:Q40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E1:E1048576"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -638,144 +638,144 @@
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="4" t="s">
+      <c r="C1" s="18"/>
+      <c r="D1" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="5"/>
-      <c r="F1" s="4" t="s">
+      <c r="E1" s="18"/>
+      <c r="F1" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="5"/>
+      <c r="G1" s="18"/>
     </row>
     <row r="2" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="10">
-        <v>8</v>
-      </c>
-      <c r="C3" s="11">
+      <c r="A3" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="8">
+        <v>8</v>
+      </c>
+      <c r="C3" s="9">
         <v>761600</v>
       </c>
-      <c r="D3" s="10">
+      <c r="D3" s="8">
         <v>88</v>
       </c>
-      <c r="E3" s="11">
+      <c r="E3" s="9">
         <v>8377600</v>
       </c>
-      <c r="F3" s="10">
+      <c r="F3" s="8">
         <v>88</v>
       </c>
-      <c r="G3" s="11">
+      <c r="G3" s="9">
         <v>8377600</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="12">
-        <v>0</v>
-      </c>
-      <c r="C4" s="11">
-        <v>0</v>
-      </c>
-      <c r="D4" s="12">
-        <v>0</v>
-      </c>
-      <c r="E4" s="11">
-        <v>0</v>
-      </c>
-      <c r="F4" s="12">
-        <v>0</v>
-      </c>
-      <c r="G4" s="11">
+      <c r="B4" s="10">
+        <v>0</v>
+      </c>
+      <c r="C4" s="9">
+        <v>0</v>
+      </c>
+      <c r="D4" s="10">
+        <v>0</v>
+      </c>
+      <c r="E4" s="9">
+        <v>0</v>
+      </c>
+      <c r="F4" s="10">
+        <v>0</v>
+      </c>
+      <c r="G4" s="9">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="12">
-        <v>0</v>
-      </c>
-      <c r="C5" s="11">
-        <v>0</v>
-      </c>
-      <c r="D5" s="12">
-        <v>0</v>
-      </c>
-      <c r="E5" s="11">
-        <v>0</v>
-      </c>
-      <c r="F5" s="12">
-        <v>0</v>
-      </c>
-      <c r="G5" s="11">
+      <c r="B5" s="10">
+        <v>0</v>
+      </c>
+      <c r="C5" s="9">
+        <v>0</v>
+      </c>
+      <c r="D5" s="10">
+        <v>0</v>
+      </c>
+      <c r="E5" s="9">
+        <v>0</v>
+      </c>
+      <c r="F5" s="10">
+        <v>0</v>
+      </c>
+      <c r="G5" s="9">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="14">
-        <v>0</v>
-      </c>
-      <c r="C6" s="15">
-        <v>0</v>
-      </c>
-      <c r="D6" s="14">
-        <v>0</v>
-      </c>
-      <c r="E6" s="15">
-        <v>0</v>
-      </c>
-      <c r="F6" s="14">
-        <v>0</v>
-      </c>
-      <c r="G6" s="15">
+      <c r="B6" s="12">
+        <v>0</v>
+      </c>
+      <c r="C6" s="13">
+        <v>0</v>
+      </c>
+      <c r="D6" s="12">
+        <v>0</v>
+      </c>
+      <c r="E6" s="13">
+        <v>0</v>
+      </c>
+      <c r="F6" s="12">
+        <v>0</v>
+      </c>
+      <c r="G6" s="13">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="17"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="18"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="16"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
@@ -792,7 +792,7 @@
         <v>42370</v>
       </c>
       <c r="C8">
-        <v>1</v>
+        <v>200000</v>
       </c>
       <c r="E8">
         <v>8</v>
@@ -1151,7 +1151,7 @@
       </c>
       <c r="C39">
         <f>SUM(C8:C19)+SUM(G8:G19)</f>
-        <v>2964</v>
+        <v>202963</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>